<commit_message>
.gitignore update and secured settings.py file
</commit_message>
<xml_diff>
--- a/media/qbreports/uploads/xlsx_to_formated_xlsx.xlsx
+++ b/media/qbreports/uploads/xlsx_to_formated_xlsx.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="142">
   <si>
     <t>Notes</t>
   </si>
@@ -57,13 +57,13 @@
     <t>Memo</t>
   </si>
   <si>
-    <t>Arthur Court Designs, Inc.</t>
-  </si>
-  <si>
-    <t>2018-11-05</t>
-  </si>
-  <si>
-    <t>859580-1</t>
+    <t>American Cover Design 26, Inc.</t>
+  </si>
+  <si>
+    <t>2019-01-24</t>
+  </si>
+  <si>
+    <t>903252-2</t>
   </si>
   <si>
     <t>5.0</t>
@@ -72,19 +72,19 @@
     <t>0.0</t>
   </si>
   <si>
-    <t>859580</t>
-  </si>
-  <si>
-    <t>125.0</t>
-  </si>
-  <si>
-    <t>-62.5</t>
+    <t>903252</t>
+  </si>
+  <si>
+    <t>21.9</t>
+  </si>
+  <si>
+    <t>-9.0</t>
   </si>
   <si>
     <t>PO MISMATCH</t>
   </si>
   <si>
-    <t>7665353-20181113180023</t>
+    <t>7859272-20190205180021</t>
   </si>
   <si>
     <t>Code</t>
@@ -102,349 +102,325 @@
     <t>Drop Ship Total</t>
   </si>
   <si>
-    <t>2CA070080</t>
-  </si>
-  <si>
-    <t>Longhorn Bamboo Carving Board</t>
+    <t>PWL3743X8</t>
+  </si>
+  <si>
+    <t>Rodeo Rug - 2 x 7</t>
   </si>
   <si>
     <t>1.0</t>
   </si>
   <si>
-    <t>62.5</t>
-  </si>
-  <si>
-    <t>2018-11-30</t>
-  </si>
-  <si>
-    <t>859580-2</t>
-  </si>
-  <si>
-    <t>7731573-20181211180027</t>
-  </si>
-  <si>
-    <t>Always Azul Pottery</t>
-  </si>
-  <si>
-    <t>2018-12-19</t>
-  </si>
-  <si>
-    <t>872932-1</t>
+    <t>Authentic Models</t>
+  </si>
+  <si>
+    <t>2019-01-15</t>
+  </si>
+  <si>
+    <t>898313-2</t>
+  </si>
+  <si>
+    <t>898313</t>
+  </si>
+  <si>
+    <t>330.0</t>
+  </si>
+  <si>
+    <t>-16.5</t>
+  </si>
+  <si>
+    <t>7811975-20190118180029</t>
+  </si>
+  <si>
+    <t>2AMFE123</t>
+  </si>
+  <si>
+    <t>Nautical Chevron Oar</t>
+  </si>
+  <si>
+    <t>69.5</t>
+  </si>
+  <si>
+    <t>2AMFE124</t>
+  </si>
+  <si>
+    <t>Nautical Star Oar</t>
+  </si>
+  <si>
+    <t>2AMFE125</t>
+  </si>
+  <si>
+    <t>Nautical Oar Number 3</t>
+  </si>
+  <si>
+    <t>2AMFE126</t>
+  </si>
+  <si>
+    <t>Nautical Stripe Oar</t>
+  </si>
+  <si>
+    <t>49.5</t>
+  </si>
+  <si>
+    <t>2AMFE127</t>
+  </si>
+  <si>
+    <t>Nautical Sailing Flag Oar</t>
+  </si>
+  <si>
+    <t>2AMFE128</t>
+  </si>
+  <si>
+    <t>Nautical Oar Rack</t>
+  </si>
+  <si>
+    <t>22.5</t>
+  </si>
+  <si>
+    <t>2019-02-05</t>
+  </si>
+  <si>
+    <t>7866880-20190208180021</t>
+  </si>
+  <si>
+    <t>Designers Fountain</t>
+  </si>
+  <si>
+    <t>2019-01-23</t>
+  </si>
+  <si>
+    <t>902618-1</t>
+  </si>
+  <si>
+    <t>902618</t>
+  </si>
+  <si>
+    <t>200.25</t>
+  </si>
+  <si>
+    <t>-66.75</t>
+  </si>
+  <si>
+    <t>7834462-20190125180026</t>
+  </si>
+  <si>
+    <t>DF97303WSD</t>
+  </si>
+  <si>
+    <t>Austin Bath Bar - 3 Light</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>66.75</t>
+  </si>
+  <si>
+    <t>HiEnd Accents</t>
+  </si>
+  <si>
+    <t>906907-1</t>
+  </si>
+  <si>
+    <t>906907</t>
+  </si>
+  <si>
+    <t>33.0</t>
+  </si>
+  <si>
+    <t>-2.0</t>
+  </si>
+  <si>
+    <t>7870202-20190208180021</t>
+  </si>
+  <si>
+    <t>2HMBS1001QNOC</t>
+  </si>
+  <si>
+    <t>Faux Leather Bedskirt - Queen</t>
+  </si>
+  <si>
+    <t>KAS Oriental Rugs, Inc.</t>
+  </si>
+  <si>
+    <t>2019-01-08</t>
+  </si>
+  <si>
+    <t>894910-1</t>
+  </si>
+  <si>
+    <t>894910</t>
+  </si>
+  <si>
+    <t>95.0</t>
+  </si>
+  <si>
+    <t>-95.0</t>
+  </si>
+  <si>
+    <t>7795476-20190111180028</t>
+  </si>
+  <si>
+    <t>2KAHAR421633X53</t>
+  </si>
+  <si>
+    <t>Rippling Waves Indoor/Outdoor Rug - 3 x 5</t>
   </si>
   <si>
     <t>2.0</t>
   </si>
   <si>
-    <t>872932</t>
-  </si>
-  <si>
-    <t>60.0</t>
-  </si>
-  <si>
-    <t>-60.0</t>
-  </si>
-  <si>
-    <t>7763335-20181225180010</t>
-  </si>
-  <si>
-    <t>AZ207ORMWMT</t>
-  </si>
-  <si>
-    <t>Mountain Moose Pottery Dinnerware - 4 pcs</t>
-  </si>
-  <si>
-    <t>2018-12-18</t>
-  </si>
-  <si>
-    <t>7807711-20190115180020</t>
-  </si>
-  <si>
-    <t>2018-12-26</t>
-  </si>
-  <si>
-    <t>888829-3</t>
-  </si>
-  <si>
-    <t>888829</t>
-  </si>
-  <si>
-    <t>29.5</t>
-  </si>
-  <si>
-    <t>-5.9</t>
-  </si>
-  <si>
-    <t>7807685-20190115180020</t>
-  </si>
-  <si>
-    <t>2CA550172</t>
-  </si>
-  <si>
-    <t>Silver Stallion Paper Towel Holder</t>
+    <t>47.5</t>
+  </si>
+  <si>
+    <t>2019-01-30</t>
+  </si>
+  <si>
+    <t>7851056-20190205180021</t>
+  </si>
+  <si>
+    <t>Kimlor</t>
+  </si>
+  <si>
+    <t>906263-4</t>
+  </si>
+  <si>
+    <t>906263</t>
+  </si>
+  <si>
+    <t>82.5</t>
+  </si>
+  <si>
+    <t>-2.25</t>
+  </si>
+  <si>
+    <t>7851083-20190205180021</t>
+  </si>
+  <si>
+    <t>Mohawk Factoring LLC</t>
+  </si>
+  <si>
+    <t>2019-02-01</t>
+  </si>
+  <si>
+    <t>907020-1</t>
+  </si>
+  <si>
+    <t>907020</t>
+  </si>
+  <si>
+    <t>558.45</t>
+  </si>
+  <si>
+    <t>-19.55</t>
+  </si>
+  <si>
+    <t>7862523-20190205180021</t>
+  </si>
+  <si>
+    <t>MO909352004412X</t>
+  </si>
+  <si>
+    <t>Amarillo Spice Rug - 12 x 15</t>
+  </si>
+  <si>
+    <t>OK CASTING, LLC.</t>
+  </si>
+  <si>
+    <t>901236-1</t>
+  </si>
+  <si>
+    <t>15.0</t>
+  </si>
+  <si>
+    <t>901236</t>
+  </si>
+  <si>
+    <t>207.0</t>
+  </si>
+  <si>
+    <t>-1.0</t>
+  </si>
+  <si>
+    <t>7851111-20190205180021</t>
+  </si>
+  <si>
+    <t>LG0353SBW</t>
+  </si>
+  <si>
+    <t>Black Forest Game Mirror</t>
+  </si>
+  <si>
+    <t>904280-1</t>
+  </si>
+  <si>
+    <t>904280</t>
+  </si>
+  <si>
+    <t>276.0</t>
+  </si>
+  <si>
+    <t>-32.0</t>
+  </si>
+  <si>
+    <t>7866938-20190208180021</t>
+  </si>
+  <si>
+    <t>LG0690CSZWL</t>
+  </si>
+  <si>
+    <t>Stag Mount Wall Sconce with Faux Leather Shade - Right Facing</t>
+  </si>
+  <si>
+    <t>138.0</t>
+  </si>
+  <si>
+    <t>LG0691CSZWL</t>
+  </si>
+  <si>
+    <t>Stag Mount Wall Sconce with Faux Leather Shade - Left Facing</t>
+  </si>
+  <si>
+    <t>WILD WINGS</t>
   </si>
   <si>
     <t>2019-01-17</t>
   </si>
   <si>
-    <t>872932-</t>
-  </si>
-  <si>
-    <t>7820552-20190118180029</t>
-  </si>
-  <si>
-    <t>Designers Fountain</t>
-  </si>
-  <si>
-    <t>2019-01-14</t>
-  </si>
-  <si>
-    <t>898375-1</t>
-  </si>
-  <si>
-    <t>898375</t>
-  </si>
-  <si>
-    <t>66.75</t>
-  </si>
-  <si>
-    <t>-3.2</t>
-  </si>
-  <si>
-    <t>7808363-20190118180029</t>
-  </si>
-  <si>
-    <t>DF97303WSD</t>
-  </si>
-  <si>
-    <t>Austin Bath Bar - 3 Light</t>
-  </si>
-  <si>
-    <t>2019-01-15</t>
-  </si>
-  <si>
-    <t>896995-1</t>
-  </si>
-  <si>
-    <t>896995</t>
-  </si>
-  <si>
-    <t>63.75</t>
-  </si>
-  <si>
-    <t>-1.2</t>
-  </si>
-  <si>
-    <t>7815790-20190118180029</t>
-  </si>
-  <si>
-    <t>DF-95603-OB</t>
-  </si>
-  <si>
-    <t>Timberline Vanity Light - 3 Light - OUT OF STOCK</t>
-  </si>
-  <si>
-    <t>897103-3</t>
-  </si>
-  <si>
-    <t>897103</t>
-  </si>
-  <si>
-    <t>7815791-20190118180029</t>
-  </si>
-  <si>
-    <t>EVERGREEN ENTERPRISES</t>
-  </si>
-  <si>
-    <t>896925-1</t>
-  </si>
-  <si>
-    <t>896925</t>
-  </si>
-  <si>
-    <t>260.0</t>
-  </si>
-  <si>
-    <t>-26.0</t>
-  </si>
-  <si>
-    <t>7815883-20190118180029</t>
-  </si>
-  <si>
-    <t>EE4S5001</t>
-  </si>
-  <si>
-    <t>Red Tractor Barstool</t>
-  </si>
-  <si>
-    <t>4.0</t>
-  </si>
-  <si>
-    <t>65.0</t>
-  </si>
-  <si>
-    <t>HiEnd Accents</t>
-  </si>
-  <si>
-    <t>2018-11-20</t>
-  </si>
-  <si>
-    <t>864953-2</t>
-  </si>
-  <si>
-    <t>864953</t>
-  </si>
-  <si>
-    <t>35.0</t>
-  </si>
-  <si>
-    <t>-5.0</t>
-  </si>
-  <si>
-    <t>7811506-20190118180029</t>
-  </si>
-  <si>
-    <t>2HMBS1001KGOC</t>
-  </si>
-  <si>
-    <t>Faux Leather Bedskirt - King</t>
-  </si>
-  <si>
-    <t>897360-2</t>
-  </si>
-  <si>
-    <t>897360</t>
-  </si>
-  <si>
-    <t>7815861-20190118180029</t>
-  </si>
-  <si>
-    <t>Lorec Ranch Wholesale</t>
-  </si>
-  <si>
-    <t>899442-</t>
-  </si>
-  <si>
-    <t>10.0</t>
-  </si>
-  <si>
-    <t>899442</t>
-  </si>
-  <si>
-    <t>34.99</t>
-  </si>
-  <si>
-    <t>7816579-20190118180029</t>
-  </si>
-  <si>
-    <t>Michaelian Home, Inc.</t>
-  </si>
-  <si>
-    <t>898580-1</t>
-  </si>
-  <si>
-    <t>898580</t>
-  </si>
-  <si>
-    <t>7815973-20190118180029</t>
-  </si>
-  <si>
-    <t>2MHNPE035</t>
-  </si>
-  <si>
-    <t>Warrior Printed Pillow</t>
-  </si>
-  <si>
-    <t>Mohawk Factoring LLC</t>
-  </si>
-  <si>
-    <t>2019-01-08</t>
-  </si>
-  <si>
-    <t>895090-1</t>
-  </si>
-  <si>
-    <t>895090</t>
-  </si>
-  <si>
-    <t>-2.55</t>
-  </si>
-  <si>
-    <t>7811533-20190118180029</t>
-  </si>
-  <si>
-    <t>MO90932801292X7</t>
-  </si>
-  <si>
-    <t>Aztec Lore Multi Rug - 2 x 7</t>
-  </si>
-  <si>
-    <t>2019-01-09</t>
-  </si>
-  <si>
-    <t>895105-1</t>
-  </si>
-  <si>
-    <t>895105</t>
-  </si>
-  <si>
-    <t>237.15</t>
-  </si>
-  <si>
-    <t>-13.6</t>
-  </si>
-  <si>
-    <t>7811534-20190118180029</t>
-  </si>
-  <si>
-    <t>MO910159012210X</t>
-  </si>
-  <si>
-    <t>Gunmetal Strata Rug - 10 x 13</t>
-  </si>
-  <si>
-    <t>OK CASTING, LLC.</t>
-  </si>
-  <si>
-    <t>889523-1</t>
-  </si>
-  <si>
-    <t>15.0</t>
-  </si>
-  <si>
-    <t>889523</t>
-  </si>
-  <si>
-    <t>636.0</t>
-  </si>
-  <si>
-    <t>-1.0</t>
-  </si>
-  <si>
-    <t>7808387-20190118180029</t>
-  </si>
-  <si>
-    <t>LG0935BL</t>
-  </si>
-  <si>
-    <t>Just Like Dad Horse Lamp with Faux Leather Shade</t>
-  </si>
-  <si>
-    <t>224.0</t>
-  </si>
-  <si>
-    <t>LG0936BL</t>
-  </si>
-  <si>
-    <t>Just Resting Horse Lamp</t>
-  </si>
-  <si>
-    <t>188.0</t>
-  </si>
-  <si>
-    <t>LG0937BL</t>
-  </si>
-  <si>
-    <t>Stay Here Horse Lamp with Faux Leather Shade</t>
+    <t>899695-4</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>899695</t>
+  </si>
+  <si>
+    <t>-9.5</t>
+  </si>
+  <si>
+    <t>7827753-20190125180026</t>
+  </si>
+  <si>
+    <t>2019-01-28</t>
+  </si>
+  <si>
+    <t>7858707-20190205180021</t>
+  </si>
+  <si>
+    <t>903682-1</t>
+  </si>
+  <si>
+    <t>903682</t>
+  </si>
+  <si>
+    <t>7858704-20190205180021</t>
+  </si>
+  <si>
+    <t>WW5373250089</t>
+  </si>
+  <si>
+    <t>Mountain Landscape Photo Collage</t>
   </si>
   <si>
     <t>Entry Date</t>
@@ -465,7 +441,7 @@
     <t>Invoice Price</t>
   </si>
   <si>
-    <t>2019-02-19</t>
+    <t>2019-02-27</t>
   </si>
 </sst>
 </file>
@@ -806,7 +782,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -866,13 +842,13 @@
         <v>14</v>
       </c>
       <c r="D2" t="n">
-        <v>350874</v>
+        <v>1197343</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
       </c>
       <c r="F2" t="n">
-        <v>67.5</v>
+        <v>35.9</v>
       </c>
       <c r="G2" t="s">
         <v>16</v>
@@ -948,7 +924,7 @@
         <v/>
       </c>
       <c r="D4" t="n">
-        <v>350874</v>
+        <v>1197343</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -966,10 +942,10 @@
         <v>30</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="K4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L4" t="n">
         <v/>
@@ -983,81 +959,81 @@
         <v/>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
         <v>32</v>
       </c>
       <c r="D5" t="n">
-        <v>355267</v>
+        <v>1811158</v>
       </c>
       <c r="E5" t="s">
         <v>33</v>
       </c>
       <c r="F5" t="n">
-        <v>67.5</v>
+        <v>271</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
         <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="K5" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="L5" t="s">
         <v>21</v>
       </c>
       <c r="M5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="n">
         <v/>
       </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>36</v>
+      <c r="B6" t="n">
+        <v/>
+      </c>
+      <c r="C6" t="n">
+        <v/>
       </c>
       <c r="D6" t="n">
-        <v>19164</v>
-      </c>
-      <c r="E6" t="s">
-        <v>37</v>
+        <v/>
+      </c>
+      <c r="E6" t="n">
+        <v/>
       </c>
       <c r="F6" t="n">
-        <v>62</v>
+        <v/>
       </c>
       <c r="G6" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="J6" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="K6" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" t="s">
-        <v>42</v>
+        <v>27</v>
+      </c>
+      <c r="L6" t="n">
+        <v/>
+      </c>
+      <c r="M6" t="n">
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1071,28 +1047,28 @@
         <v/>
       </c>
       <c r="D7" t="n">
-        <v/>
-      </c>
-      <c r="E7" t="n">
-        <v/>
+        <v>1811158</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
       </c>
       <c r="F7" t="n">
         <v/>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="I7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J7" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="K7" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="L7" t="n">
         <v/>
@@ -1112,19 +1088,19 @@
         <v/>
       </c>
       <c r="D8" t="n">
-        <v>19164</v>
+        <v>1811158</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F8" t="n">
         <v/>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I8" t="s">
         <v>30</v>
@@ -1146,82 +1122,82 @@
       <c r="A9" t="n">
         <v/>
       </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
+      <c r="B9" t="n">
+        <v/>
+      </c>
+      <c r="C9" t="n">
+        <v/>
       </c>
       <c r="D9" t="n">
-        <v>359868</v>
+        <v>1811158</v>
       </c>
       <c r="E9" t="s">
         <v>33</v>
       </c>
       <c r="F9" t="n">
-        <v>62.5</v>
+        <v/>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="H9" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="J9" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="K9" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" t="s">
-        <v>46</v>
+        <v>40</v>
+      </c>
+      <c r="L9" t="n">
+        <v/>
+      </c>
+      <c r="M9" t="n">
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="n">
         <v/>
       </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" t="n">
+        <v/>
+      </c>
+      <c r="C10" t="n">
+        <v/>
+      </c>
+      <c r="D10" t="n">
+        <v>1811158</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="n">
+        <v/>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" t="s">
         <v>47</v>
       </c>
-      <c r="D10" t="n">
-        <v>361328</v>
-      </c>
-      <c r="E10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" t="n">
-        <v>35.4</v>
-      </c>
-      <c r="G10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" t="s">
-        <v>49</v>
-      </c>
-      <c r="J10" t="s">
-        <v>50</v>
-      </c>
       <c r="K10" t="s">
-        <v>51</v>
-      </c>
-      <c r="L10" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" t="s">
-        <v>52</v>
+        <v>47</v>
+      </c>
+      <c r="L10" t="n">
+        <v/>
+      </c>
+      <c r="M10" t="n">
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1235,28 +1211,28 @@
         <v/>
       </c>
       <c r="D11" t="n">
-        <v/>
-      </c>
-      <c r="E11" t="n">
-        <v/>
+        <v>1811158</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
       </c>
       <c r="F11" t="n">
         <v/>
       </c>
       <c r="G11" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="I11" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J11" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="K11" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="L11" t="n">
         <v/>
@@ -1276,28 +1252,28 @@
         <v/>
       </c>
       <c r="D12" t="n">
-        <v>361328</v>
+        <v>1811158</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="F12" t="n">
         <v/>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I12" t="s">
         <v>30</v>
       </c>
       <c r="J12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L12" t="n">
         <v/>
@@ -1311,81 +1287,81 @@
         <v/>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D13" t="n">
-        <v>19222</v>
+        <v>1811698</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="F13" t="n">
-        <v>62</v>
+        <v>75.5</v>
       </c>
       <c r="G13" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="H13" t="s">
         <v>17</v>
       </c>
       <c r="I13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="K13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="L13" t="s">
         <v>21</v>
       </c>
       <c r="M13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="n">
         <v/>
       </c>
-      <c r="B14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" t="s">
-        <v>59</v>
+      <c r="B14" t="n">
+        <v/>
+      </c>
+      <c r="C14" t="n">
+        <v/>
       </c>
       <c r="D14" t="n">
-        <v>93006620</v>
-      </c>
-      <c r="E14" t="s">
-        <v>60</v>
+        <v/>
+      </c>
+      <c r="E14" t="n">
+        <v/>
       </c>
       <c r="F14" t="n">
-        <v>74.95</v>
+        <v/>
       </c>
       <c r="G14" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="H14" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I14" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="J14" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="K14" t="s">
-        <v>63</v>
-      </c>
-      <c r="L14" t="s">
-        <v>21</v>
-      </c>
-      <c r="M14" t="s">
-        <v>64</v>
+        <v>27</v>
+      </c>
+      <c r="L14" t="n">
+        <v/>
+      </c>
+      <c r="M14" t="n">
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1399,28 +1375,28 @@
         <v/>
       </c>
       <c r="D15" t="n">
-        <v/>
-      </c>
-      <c r="E15" t="n">
-        <v/>
+        <v>1811698</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
       </c>
       <c r="F15" t="n">
         <v/>
       </c>
       <c r="G15" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H15" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="I15" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J15" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="K15" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="L15" t="n">
         <v/>
@@ -1440,28 +1416,28 @@
         <v/>
       </c>
       <c r="D16" t="n">
-        <v>93006620</v>
+        <v>1811698</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="F16" t="n">
         <v/>
       </c>
       <c r="G16" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="I16" t="s">
         <v>30</v>
       </c>
       <c r="J16" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="K16" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="L16" t="n">
         <v/>
@@ -1474,41 +1450,41 @@
       <c r="A17" t="n">
         <v/>
       </c>
-      <c r="B17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" t="s">
-        <v>67</v>
+      <c r="B17" t="n">
+        <v/>
+      </c>
+      <c r="C17" t="n">
+        <v/>
       </c>
       <c r="D17" t="n">
-        <v>93007064</v>
+        <v>1811698</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="F17" t="n">
-        <v>69.95</v>
+        <v/>
       </c>
       <c r="G17" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="H17" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="I17" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="J17" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="K17" t="s">
-        <v>71</v>
-      </c>
-      <c r="L17" t="s">
-        <v>21</v>
-      </c>
-      <c r="M17" t="s">
-        <v>72</v>
+        <v>40</v>
+      </c>
+      <c r="L17" t="n">
+        <v/>
+      </c>
+      <c r="M17" t="n">
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1522,28 +1498,28 @@
         <v/>
       </c>
       <c r="D18" t="n">
-        <v/>
-      </c>
-      <c r="E18" t="n">
-        <v/>
+        <v>1811698</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
       </c>
       <c r="F18" t="n">
         <v/>
       </c>
       <c r="G18" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="H18" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="I18" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J18" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="K18" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="L18" t="n">
         <v/>
@@ -1563,28 +1539,28 @@
         <v/>
       </c>
       <c r="D19" t="n">
-        <v>93007064</v>
+        <v>1811698</v>
       </c>
       <c r="E19" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="F19" t="n">
         <v/>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="H19" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="I19" t="s">
         <v>30</v>
       </c>
       <c r="J19" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="K19" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="L19" t="n">
         <v/>
@@ -1597,82 +1573,82 @@
       <c r="A20" t="n">
         <v/>
       </c>
-      <c r="B20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" t="s">
-        <v>67</v>
+      <c r="B20" t="n">
+        <v/>
+      </c>
+      <c r="C20" t="n">
+        <v/>
       </c>
       <c r="D20" t="n">
-        <v>93007065</v>
+        <v>1811698</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="F20" t="n">
-        <v>69.95</v>
+        <v/>
       </c>
       <c r="G20" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="H20" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="I20" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="J20" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="K20" t="s">
-        <v>71</v>
-      </c>
-      <c r="L20" t="s">
-        <v>21</v>
-      </c>
-      <c r="M20" t="s">
-        <v>77</v>
+        <v>52</v>
+      </c>
+      <c r="L20" t="n">
+        <v/>
+      </c>
+      <c r="M20" t="n">
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="n">
         <v/>
       </c>
-      <c r="B21" t="n">
-        <v/>
-      </c>
-      <c r="C21" t="n">
-        <v/>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
       </c>
       <c r="D21" t="n">
-        <v/>
-      </c>
-      <c r="E21" t="n">
-        <v/>
+        <v>93009368</v>
+      </c>
+      <c r="E21" t="s">
+        <v>57</v>
       </c>
       <c r="F21" t="n">
-        <v/>
+        <v>205.25</v>
       </c>
       <c r="G21" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="H21" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="I21" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="J21" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="K21" t="s">
-        <v>27</v>
-      </c>
-      <c r="L21" t="n">
-        <v/>
-      </c>
-      <c r="M21" t="n">
-        <v/>
+        <v>60</v>
+      </c>
+      <c r="L21" t="s">
+        <v>21</v>
+      </c>
+      <c r="M21" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -1686,28 +1662,28 @@
         <v/>
       </c>
       <c r="D22" t="n">
-        <v>93007065</v>
-      </c>
-      <c r="E22" t="s">
-        <v>75</v>
+        <v/>
+      </c>
+      <c r="E22" t="n">
+        <v/>
       </c>
       <c r="F22" t="n">
         <v/>
       </c>
       <c r="G22" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="H22" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="I22" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J22" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="K22" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="L22" t="n">
         <v/>
@@ -1720,82 +1696,82 @@
       <c r="A23" t="n">
         <v/>
       </c>
-      <c r="B23" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" t="s">
-        <v>67</v>
+      <c r="B23" t="n">
+        <v/>
+      </c>
+      <c r="C23" t="n">
+        <v/>
       </c>
       <c r="D23" t="n">
-        <v>6733751</v>
+        <v>93009368</v>
       </c>
       <c r="E23" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="F23" t="n">
-        <v>291</v>
+        <v/>
       </c>
       <c r="G23" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="H23" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="I23" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="J23" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="K23" t="s">
-        <v>82</v>
-      </c>
-      <c r="L23" t="s">
-        <v>21</v>
-      </c>
-      <c r="M23" t="s">
-        <v>83</v>
+        <v>59</v>
+      </c>
+      <c r="L23" t="n">
+        <v/>
+      </c>
+      <c r="M23" t="n">
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="n">
         <v/>
       </c>
-      <c r="B24" t="n">
-        <v/>
-      </c>
-      <c r="C24" t="n">
-        <v/>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" t="s">
+        <v>53</v>
       </c>
       <c r="D24" t="n">
-        <v/>
-      </c>
-      <c r="E24" t="n">
-        <v/>
+        <v>267008</v>
+      </c>
+      <c r="E24" t="s">
+        <v>67</v>
       </c>
       <c r="F24" t="n">
-        <v/>
+        <v>40</v>
       </c>
       <c r="G24" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="H24" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="I24" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="J24" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="K24" t="s">
-        <v>27</v>
-      </c>
-      <c r="L24" t="n">
-        <v/>
-      </c>
-      <c r="M24" t="n">
-        <v/>
+        <v>70</v>
+      </c>
+      <c r="L24" t="s">
+        <v>21</v>
+      </c>
+      <c r="M24" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -1809,28 +1785,28 @@
         <v/>
       </c>
       <c r="D25" t="n">
-        <v>6733751</v>
-      </c>
-      <c r="E25" t="s">
-        <v>79</v>
+        <v/>
+      </c>
+      <c r="E25" t="n">
+        <v/>
       </c>
       <c r="F25" t="n">
         <v/>
       </c>
       <c r="G25" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="H25" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="I25" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="J25" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="K25" t="s">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="L25" t="n">
         <v/>
@@ -1843,82 +1819,82 @@
       <c r="A26" t="n">
         <v/>
       </c>
-      <c r="B26" t="s">
-        <v>88</v>
-      </c>
-      <c r="C26" t="s">
-        <v>89</v>
+      <c r="B26" t="n">
+        <v/>
+      </c>
+      <c r="C26" t="n">
+        <v/>
       </c>
       <c r="D26" t="n">
-        <v>258738</v>
+        <v>267008</v>
       </c>
       <c r="E26" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="F26" t="n">
-        <v>45</v>
+        <v/>
       </c>
       <c r="G26" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="H26" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="I26" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
       <c r="J26" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="K26" t="s">
-        <v>93</v>
-      </c>
-      <c r="L26" t="s">
-        <v>21</v>
-      </c>
-      <c r="M26" t="s">
-        <v>94</v>
+        <v>69</v>
+      </c>
+      <c r="L26" t="n">
+        <v/>
+      </c>
+      <c r="M26" t="n">
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" t="n">
         <v/>
       </c>
-      <c r="B27" t="n">
-        <v/>
-      </c>
-      <c r="C27" t="n">
-        <v/>
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" t="s">
+        <v>75</v>
       </c>
       <c r="D27" t="n">
-        <v/>
-      </c>
-      <c r="E27" t="n">
-        <v/>
+        <v>746877</v>
+      </c>
+      <c r="E27" t="s">
+        <v>76</v>
       </c>
       <c r="F27" t="n">
-        <v/>
+        <v>95</v>
       </c>
       <c r="G27" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H27" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="I27" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="J27" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="K27" t="s">
-        <v>27</v>
-      </c>
-      <c r="L27" t="n">
-        <v/>
-      </c>
-      <c r="M27" t="n">
-        <v/>
+        <v>79</v>
+      </c>
+      <c r="L27" t="s">
+        <v>21</v>
+      </c>
+      <c r="M27" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -1932,28 +1908,28 @@
         <v/>
       </c>
       <c r="D28" t="n">
-        <v>258738</v>
-      </c>
-      <c r="E28" t="s">
-        <v>90</v>
+        <v/>
+      </c>
+      <c r="E28" t="n">
+        <v/>
       </c>
       <c r="F28" t="n">
         <v/>
       </c>
       <c r="G28" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
       <c r="H28" t="s">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="I28" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J28" t="s">
-        <v>92</v>
+        <v>26</v>
       </c>
       <c r="K28" t="s">
-        <v>92</v>
+        <v>27</v>
       </c>
       <c r="L28" t="n">
         <v/>
@@ -1966,82 +1942,82 @@
       <c r="A29" t="n">
         <v/>
       </c>
-      <c r="B29" t="s">
-        <v>88</v>
-      </c>
-      <c r="C29" t="s">
-        <v>67</v>
+      <c r="B29" t="n">
+        <v/>
+      </c>
+      <c r="C29" t="n">
+        <v/>
       </c>
       <c r="D29" t="n">
-        <v>264906</v>
+        <v>746877</v>
       </c>
       <c r="E29" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="F29" t="n">
-        <v>45</v>
+        <v/>
       </c>
       <c r="G29" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="H29" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="I29" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="J29" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="K29" t="s">
-        <v>93</v>
-      </c>
-      <c r="L29" t="s">
-        <v>21</v>
-      </c>
-      <c r="M29" t="s">
-        <v>99</v>
+        <v>78</v>
+      </c>
+      <c r="L29" t="n">
+        <v/>
+      </c>
+      <c r="M29" t="n">
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" t="n">
         <v/>
       </c>
-      <c r="B30" t="n">
-        <v/>
-      </c>
-      <c r="C30" t="n">
-        <v/>
+      <c r="B30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" t="s">
+        <v>85</v>
       </c>
       <c r="D30" t="n">
-        <v/>
-      </c>
-      <c r="E30" t="n">
-        <v/>
+        <v>751370</v>
+      </c>
+      <c r="E30" t="s">
+        <v>76</v>
       </c>
       <c r="F30" t="n">
-        <v/>
+        <v>95</v>
       </c>
       <c r="G30" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H30" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="I30" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="J30" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="K30" t="s">
-        <v>27</v>
-      </c>
-      <c r="L30" t="n">
-        <v/>
-      </c>
-      <c r="M30" t="n">
-        <v/>
+        <v>79</v>
+      </c>
+      <c r="L30" t="s">
+        <v>21</v>
+      </c>
+      <c r="M30" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -2055,28 +2031,28 @@
         <v/>
       </c>
       <c r="D31" t="n">
-        <v>264906</v>
-      </c>
-      <c r="E31" t="s">
-        <v>97</v>
+        <v/>
+      </c>
+      <c r="E31" t="n">
+        <v/>
       </c>
       <c r="F31" t="n">
         <v/>
       </c>
       <c r="G31" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
       <c r="H31" t="s">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="I31" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J31" t="s">
-        <v>92</v>
+        <v>26</v>
       </c>
       <c r="K31" t="s">
-        <v>92</v>
+        <v>27</v>
       </c>
       <c r="L31" t="n">
         <v/>
@@ -2089,41 +2065,41 @@
       <c r="A32" t="n">
         <v/>
       </c>
-      <c r="B32" t="s">
-        <v>100</v>
-      </c>
-      <c r="C32" t="s">
-        <v>55</v>
+      <c r="B32" t="n">
+        <v/>
+      </c>
+      <c r="C32" t="n">
+        <v/>
       </c>
       <c r="D32" t="n">
-        <v>923</v>
+        <v>751370</v>
       </c>
       <c r="E32" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="F32" t="n">
-        <v>49.99</v>
+        <v/>
       </c>
       <c r="G32" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="H32" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="I32" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="J32" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="K32" t="s">
-        <v>93</v>
-      </c>
-      <c r="L32" t="s">
-        <v>21</v>
-      </c>
-      <c r="M32" t="s">
-        <v>105</v>
+        <v>78</v>
+      </c>
+      <c r="L32" t="n">
+        <v/>
+      </c>
+      <c r="M32" t="n">
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -2131,81 +2107,81 @@
         <v/>
       </c>
       <c r="B33" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="D33" t="n">
-        <v>57693</v>
+        <v>883311</v>
       </c>
       <c r="E33" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="F33" t="n">
-        <v>40</v>
+        <v>87.75</v>
       </c>
       <c r="G33" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="H33" t="s">
         <v>17</v>
       </c>
       <c r="I33" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="J33" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L33" t="s">
         <v>21</v>
       </c>
       <c r="M33" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" t="n">
         <v/>
       </c>
-      <c r="B34" t="n">
-        <v/>
-      </c>
-      <c r="C34" t="n">
-        <v/>
+      <c r="B34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" t="s">
+        <v>94</v>
       </c>
       <c r="D34" t="n">
-        <v/>
-      </c>
-      <c r="E34" t="n">
-        <v/>
+        <v>9683149</v>
+      </c>
+      <c r="E34" t="s">
+        <v>95</v>
       </c>
       <c r="F34" t="n">
-        <v/>
+        <v>578</v>
       </c>
       <c r="G34" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H34" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="I34" t="s">
-        <v>25</v>
+        <v>96</v>
       </c>
       <c r="J34" t="s">
-        <v>26</v>
+        <v>97</v>
       </c>
       <c r="K34" t="s">
-        <v>27</v>
-      </c>
-      <c r="L34" t="n">
-        <v/>
-      </c>
-      <c r="M34" t="n">
-        <v/>
+        <v>98</v>
+      </c>
+      <c r="L34" t="s">
+        <v>21</v>
+      </c>
+      <c r="M34" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -2219,28 +2195,28 @@
         <v/>
       </c>
       <c r="D35" t="n">
-        <v>57693</v>
-      </c>
-      <c r="E35" t="s">
-        <v>107</v>
+        <v/>
+      </c>
+      <c r="E35" t="n">
+        <v/>
       </c>
       <c r="F35" t="n">
         <v/>
       </c>
       <c r="G35" t="s">
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="H35" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="I35" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J35" t="s">
-        <v>92</v>
+        <v>26</v>
       </c>
       <c r="K35" t="s">
-        <v>92</v>
+        <v>27</v>
       </c>
       <c r="L35" t="n">
         <v/>
@@ -2253,82 +2229,82 @@
       <c r="A36" t="n">
         <v/>
       </c>
-      <c r="B36" t="s">
-        <v>112</v>
-      </c>
-      <c r="C36" t="s">
-        <v>113</v>
+      <c r="B36" t="n">
+        <v/>
+      </c>
+      <c r="C36" t="n">
+        <v/>
       </c>
       <c r="D36" t="n">
-        <v>9592522</v>
+        <v>9683149</v>
       </c>
       <c r="E36" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="F36" t="n">
-        <v>66.3</v>
+        <v/>
       </c>
       <c r="G36" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="H36" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="I36" t="s">
-        <v>115</v>
+        <v>30</v>
       </c>
       <c r="J36" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="K36" t="s">
-        <v>116</v>
-      </c>
-      <c r="L36" t="s">
-        <v>21</v>
-      </c>
-      <c r="M36" t="s">
-        <v>117</v>
+        <v>97</v>
+      </c>
+      <c r="L36" t="n">
+        <v/>
+      </c>
+      <c r="M36" t="n">
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" t="n">
         <v/>
       </c>
-      <c r="B37" t="n">
-        <v/>
-      </c>
-      <c r="C37" t="n">
-        <v/>
+      <c r="B37" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" t="s">
+        <v>85</v>
       </c>
       <c r="D37" t="n">
-        <v/>
-      </c>
-      <c r="E37" t="n">
-        <v/>
+        <v>69741</v>
+      </c>
+      <c r="E37" t="s">
+        <v>103</v>
       </c>
       <c r="F37" t="n">
-        <v/>
+        <v>223</v>
       </c>
       <c r="G37" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="H37" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="I37" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
       <c r="J37" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="K37" t="s">
-        <v>27</v>
-      </c>
-      <c r="L37" t="n">
-        <v/>
-      </c>
-      <c r="M37" t="n">
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="L37" t="s">
+        <v>21</v>
+      </c>
+      <c r="M37" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -2342,28 +2318,28 @@
         <v/>
       </c>
       <c r="D38" t="n">
-        <v>9592522</v>
-      </c>
-      <c r="E38" t="s">
-        <v>114</v>
+        <v/>
+      </c>
+      <c r="E38" t="n">
+        <v/>
       </c>
       <c r="F38" t="n">
         <v/>
       </c>
       <c r="G38" t="s">
-        <v>118</v>
+        <v>23</v>
       </c>
       <c r="H38" t="s">
-        <v>119</v>
+        <v>24</v>
       </c>
       <c r="I38" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J38" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="K38" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="L38" t="n">
         <v/>
@@ -2376,82 +2352,82 @@
       <c r="A39" t="n">
         <v/>
       </c>
-      <c r="B39" t="s">
-        <v>112</v>
-      </c>
-      <c r="C39" t="s">
-        <v>120</v>
+      <c r="B39" t="n">
+        <v/>
+      </c>
+      <c r="C39" t="n">
+        <v/>
       </c>
       <c r="D39" t="n">
-        <v>9596769</v>
+        <v>69741</v>
       </c>
       <c r="E39" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="F39" t="n">
-        <v>250.75</v>
+        <v/>
       </c>
       <c r="G39" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="H39" t="s">
-        <v>17</v>
+        <v>110</v>
       </c>
       <c r="I39" t="s">
-        <v>122</v>
+        <v>30</v>
       </c>
       <c r="J39" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="K39" t="s">
-        <v>124</v>
-      </c>
-      <c r="L39" t="s">
-        <v>21</v>
-      </c>
-      <c r="M39" t="s">
-        <v>125</v>
+        <v>106</v>
+      </c>
+      <c r="L39" t="n">
+        <v/>
+      </c>
+      <c r="M39" t="n">
+        <v/>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" t="n">
         <v/>
       </c>
-      <c r="B40" t="n">
-        <v/>
-      </c>
-      <c r="C40" t="n">
-        <v/>
+      <c r="B40" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" t="s">
+        <v>53</v>
       </c>
       <c r="D40" t="n">
-        <v/>
-      </c>
-      <c r="E40" t="n">
-        <v/>
+        <v>69759</v>
+      </c>
+      <c r="E40" t="s">
+        <v>111</v>
       </c>
       <c r="F40" t="n">
-        <v/>
+        <v>323</v>
       </c>
       <c r="G40" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="H40" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="I40" t="s">
-        <v>25</v>
+        <v>112</v>
       </c>
       <c r="J40" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="K40" t="s">
-        <v>27</v>
-      </c>
-      <c r="L40" t="n">
-        <v/>
-      </c>
-      <c r="M40" t="n">
-        <v/>
+        <v>114</v>
+      </c>
+      <c r="L40" t="s">
+        <v>21</v>
+      </c>
+      <c r="M40" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -2465,28 +2441,28 @@
         <v/>
       </c>
       <c r="D41" t="n">
-        <v>9596769</v>
-      </c>
-      <c r="E41" t="s">
-        <v>121</v>
+        <v/>
+      </c>
+      <c r="E41" t="n">
+        <v/>
       </c>
       <c r="F41" t="n">
         <v/>
       </c>
       <c r="G41" t="s">
-        <v>126</v>
+        <v>23</v>
       </c>
       <c r="H41" t="s">
-        <v>127</v>
+        <v>24</v>
       </c>
       <c r="I41" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J41" t="s">
-        <v>123</v>
+        <v>26</v>
       </c>
       <c r="K41" t="s">
-        <v>123</v>
+        <v>27</v>
       </c>
       <c r="L41" t="n">
         <v/>
@@ -2499,41 +2475,41 @@
       <c r="A42" t="n">
         <v/>
       </c>
-      <c r="B42" t="s">
-        <v>128</v>
-      </c>
-      <c r="C42" t="s">
-        <v>59</v>
+      <c r="B42" t="n">
+        <v/>
+      </c>
+      <c r="C42" t="n">
+        <v/>
       </c>
       <c r="D42" t="n">
-        <v>69654</v>
+        <v>69759</v>
       </c>
       <c r="E42" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="F42" t="n">
-        <v>652</v>
+        <v/>
       </c>
       <c r="G42" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="H42" t="s">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="I42" t="s">
-        <v>131</v>
+        <v>30</v>
       </c>
       <c r="J42" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="K42" t="s">
-        <v>133</v>
-      </c>
-      <c r="L42" t="s">
-        <v>21</v>
-      </c>
-      <c r="M42" t="s">
-        <v>134</v>
+        <v>118</v>
+      </c>
+      <c r="L42" t="n">
+        <v/>
+      </c>
+      <c r="M42" t="n">
+        <v/>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -2547,28 +2523,28 @@
         <v/>
       </c>
       <c r="D43" t="n">
-        <v/>
-      </c>
-      <c r="E43" t="n">
-        <v/>
+        <v>69759</v>
+      </c>
+      <c r="E43" t="s">
+        <v>111</v>
       </c>
       <c r="F43" t="n">
         <v/>
       </c>
       <c r="G43" t="s">
-        <v>23</v>
+        <v>119</v>
       </c>
       <c r="H43" t="s">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="I43" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J43" t="s">
-        <v>26</v>
+        <v>118</v>
       </c>
       <c r="K43" t="s">
-        <v>27</v>
+        <v>118</v>
       </c>
       <c r="L43" t="n">
         <v/>
@@ -2581,122 +2557,204 @@
       <c r="A44" t="n">
         <v/>
       </c>
-      <c r="B44" t="n">
-        <v/>
-      </c>
-      <c r="C44" t="n">
-        <v/>
+      <c r="B44" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" t="s">
+        <v>122</v>
       </c>
       <c r="D44" t="n">
-        <v>69654</v>
+        <v>359675</v>
       </c>
       <c r="E44" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F44" t="n">
-        <v/>
+        <v>50</v>
       </c>
       <c r="G44" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H44" t="s">
-        <v>136</v>
+        <v>17</v>
       </c>
       <c r="I44" t="s">
-        <v>30</v>
+        <v>125</v>
       </c>
       <c r="J44" t="s">
-        <v>137</v>
+        <v>78</v>
       </c>
       <c r="K44" t="s">
-        <v>137</v>
-      </c>
-      <c r="L44" t="n">
-        <v/>
-      </c>
-      <c r="M44" t="n">
-        <v/>
+        <v>126</v>
+      </c>
+      <c r="L44" t="s">
+        <v>21</v>
+      </c>
+      <c r="M44" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" t="n">
         <v/>
       </c>
-      <c r="B45" t="n">
-        <v/>
-      </c>
-      <c r="C45" t="n">
-        <v/>
+      <c r="B45" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45" t="s">
+        <v>128</v>
       </c>
       <c r="D45" t="n">
-        <v>69654</v>
+        <v>360414</v>
       </c>
       <c r="E45" t="s">
+        <v>123</v>
+      </c>
+      <c r="F45" t="n">
+        <v>59.5</v>
+      </c>
+      <c r="G45" t="s">
+        <v>124</v>
+      </c>
+      <c r="H45" t="s">
+        <v>17</v>
+      </c>
+      <c r="I45" t="s">
+        <v>125</v>
+      </c>
+      <c r="J45" t="s">
+        <v>78</v>
+      </c>
+      <c r="K45" t="s">
+        <v>126</v>
+      </c>
+      <c r="L45" t="s">
+        <v>21</v>
+      </c>
+      <c r="M45" t="s">
         <v>129</v>
-      </c>
-      <c r="F45" t="n">
-        <v/>
-      </c>
-      <c r="G45" t="s">
-        <v>138</v>
-      </c>
-      <c r="H45" t="s">
-        <v>139</v>
-      </c>
-      <c r="I45" t="s">
-        <v>30</v>
-      </c>
-      <c r="J45" t="s">
-        <v>140</v>
-      </c>
-      <c r="K45" t="s">
-        <v>140</v>
-      </c>
-      <c r="L45" t="n">
-        <v/>
-      </c>
-      <c r="M45" t="n">
-        <v/>
       </c>
     </row>
     <row r="46" spans="1:13">
       <c r="A46" t="n">
         <v/>
       </c>
-      <c r="B46" t="n">
-        <v/>
-      </c>
-      <c r="C46" t="n">
-        <v/>
+      <c r="B46" t="s">
+        <v>121</v>
+      </c>
+      <c r="C46" t="s">
+        <v>128</v>
       </c>
       <c r="D46" t="n">
-        <v>69654</v>
+        <v>360387</v>
       </c>
       <c r="E46" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F46" t="n">
-        <v/>
+        <v>59.5</v>
       </c>
       <c r="G46" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="H46" t="s">
-        <v>142</v>
+        <v>17</v>
       </c>
       <c r="I46" t="s">
+        <v>131</v>
+      </c>
+      <c r="J46" t="s">
+        <v>84</v>
+      </c>
+      <c r="K46" t="s">
+        <v>126</v>
+      </c>
+      <c r="L46" t="s">
+        <v>21</v>
+      </c>
+      <c r="M46" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" t="n">
+        <v/>
+      </c>
+      <c r="B47" t="n">
+        <v/>
+      </c>
+      <c r="C47" t="n">
+        <v/>
+      </c>
+      <c r="D47" t="n">
+        <v/>
+      </c>
+      <c r="E47" t="n">
+        <v/>
+      </c>
+      <c r="F47" t="n">
+        <v/>
+      </c>
+      <c r="G47" t="s">
+        <v>23</v>
+      </c>
+      <c r="H47" t="s">
+        <v>24</v>
+      </c>
+      <c r="I47" t="s">
+        <v>25</v>
+      </c>
+      <c r="J47" t="s">
+        <v>26</v>
+      </c>
+      <c r="K47" t="s">
+        <v>27</v>
+      </c>
+      <c r="L47" t="n">
+        <v/>
+      </c>
+      <c r="M47" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" t="n">
+        <v/>
+      </c>
+      <c r="B48" t="n">
+        <v/>
+      </c>
+      <c r="C48" t="n">
+        <v/>
+      </c>
+      <c r="D48" t="n">
+        <v>360387</v>
+      </c>
+      <c r="E48" t="s">
+        <v>130</v>
+      </c>
+      <c r="F48" t="n">
+        <v/>
+      </c>
+      <c r="G48" t="s">
+        <v>133</v>
+      </c>
+      <c r="H48" t="s">
+        <v>134</v>
+      </c>
+      <c r="I48" t="s">
         <v>30</v>
       </c>
-      <c r="J46" t="s">
-        <v>137</v>
-      </c>
-      <c r="K46" t="s">
-        <v>137</v>
-      </c>
-      <c r="L46" t="n">
-        <v/>
-      </c>
-      <c r="M46" t="n">
+      <c r="J48" t="s">
+        <v>84</v>
+      </c>
+      <c r="K48" t="s">
+        <v>84</v>
+      </c>
+      <c r="L48" t="n">
+        <v/>
+      </c>
+      <c r="M48" t="n">
         <v/>
       </c>
     </row>
@@ -2711,7 +2769,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2724,7 +2782,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2733,19 +2791,19 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="G1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="H1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2753,16 +2811,16 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="n">
-        <v>350874</v>
+        <v>1197343</v>
       </c>
       <c r="E2" t="n">
-        <v>859580</v>
+        <v>903252</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
@@ -2771,416 +2829,619 @@
         <v>28</v>
       </c>
       <c r="H2" t="n">
-        <v>62.5</v>
+        <v>21.9</v>
       </c>
       <c r="I2" t="n">
-        <v>67.5</v>
+        <v>35.9</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D3" t="n">
-        <v>19164</v>
+        <v>1811158</v>
       </c>
       <c r="E3" t="n">
-        <v>872932</v>
+        <v>898313</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H3" t="n">
-        <v>60</v>
+        <v>69.5</v>
       </c>
       <c r="I3" t="n">
-        <v>62</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D4" t="n">
-        <v>361328</v>
+        <v>1811158</v>
       </c>
       <c r="E4" t="n">
-        <v>888829</v>
+        <v>898313</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="H4" t="n">
-        <v>29.5</v>
+        <v>69.5</v>
       </c>
       <c r="I4" t="n">
-        <v>35.4</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="D5" t="n">
-        <v>93006620</v>
+        <v>1811158</v>
       </c>
       <c r="E5" t="n">
-        <v>898375</v>
+        <v>898313</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="H5" t="n">
-        <v>66.75</v>
+        <v>69.5</v>
       </c>
       <c r="I5" t="n">
-        <v>74.95</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="D6" t="n">
-        <v>93007064</v>
+        <v>1811158</v>
       </c>
       <c r="E6" t="n">
-        <v>896995</v>
+        <v>898313</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="H6" t="n">
-        <v>63.75</v>
+        <v>49.5</v>
       </c>
       <c r="I6" t="n">
-        <v>69.95</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="D7" t="n">
-        <v>93007065</v>
+        <v>1811158</v>
       </c>
       <c r="E7" t="n">
-        <v>897103</v>
+        <v>898313</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="H7" t="n">
-        <v>63.75</v>
+        <v>49.5</v>
       </c>
       <c r="I7" t="n">
-        <v>69.95</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="D8" t="n">
-        <v>6733751</v>
+        <v>1811158</v>
       </c>
       <c r="E8" t="n">
-        <v>896925</v>
+        <v>898313</v>
       </c>
       <c r="F8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="H8" t="n">
-        <v>65</v>
+        <v>22.5</v>
       </c>
       <c r="I8" t="n">
-        <v>291</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="D9" t="n">
-        <v>258738</v>
+        <v>1811698</v>
       </c>
       <c r="E9" t="n">
-        <v>864953</v>
+        <v>898313</v>
       </c>
       <c r="F9" t="n">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>95</v>
+        <v>38</v>
       </c>
       <c r="H9" t="n">
-        <v>35</v>
+        <v>69.5</v>
       </c>
       <c r="I9" t="n">
-        <v>45</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D10" t="n">
-        <v>264906</v>
+        <v>1811698</v>
       </c>
       <c r="E10" t="n">
-        <v>897360</v>
+        <v>898313</v>
       </c>
       <c r="F10" t="n">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>95</v>
+        <v>41</v>
       </c>
       <c r="H10" t="n">
-        <v>35</v>
+        <v>69.5</v>
       </c>
       <c r="I10" t="n">
-        <v>45</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D11" t="n">
-        <v>57693</v>
+        <v>1811698</v>
       </c>
       <c r="E11" t="n">
-        <v>898580</v>
+        <v>898313</v>
       </c>
       <c r="F11" t="n">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="H11" t="n">
-        <v>35</v>
+        <v>69.5</v>
       </c>
       <c r="I11" t="n">
-        <v>40</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>112</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="D12" t="n">
-        <v>9592522</v>
+        <v>1811698</v>
       </c>
       <c r="E12" t="n">
-        <v>895090</v>
+        <v>898313</v>
       </c>
       <c r="F12" t="n">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="H12" t="n">
-        <v>63.75</v>
+        <v>49.5</v>
       </c>
       <c r="I12" t="n">
-        <v>66.3</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C13" t="s">
-        <v>120</v>
+        <v>53</v>
       </c>
       <c r="D13" t="n">
-        <v>9596769</v>
+        <v>1811698</v>
       </c>
       <c r="E13" t="n">
-        <v>895105</v>
+        <v>898313</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>126</v>
+        <v>48</v>
       </c>
       <c r="H13" t="n">
-        <v>237.15</v>
+        <v>49.5</v>
       </c>
       <c r="I13" t="n">
-        <v>250.75</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>128</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D14" t="n">
-        <v>69654</v>
+        <v>1811698</v>
       </c>
       <c r="E14" t="n">
-        <v>889523</v>
+        <v>898313</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>135</v>
+        <v>50</v>
       </c>
       <c r="H14" t="n">
-        <v>224</v>
+        <v>22.5</v>
       </c>
       <c r="I14" t="n">
-        <v>652</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D15" t="n">
-        <v>69654</v>
+        <v>93009368</v>
       </c>
       <c r="E15" t="n">
-        <v>889523</v>
+        <v>902618</v>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G15" t="s">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="H15" t="n">
-        <v>188</v>
+        <v>66.75</v>
       </c>
       <c r="I15" t="n">
-        <v>652</v>
+        <v>205.25</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D16" t="n">
-        <v>69654</v>
+        <v>267008</v>
       </c>
       <c r="E16" t="n">
-        <v>889523</v>
+        <v>906907</v>
       </c>
       <c r="F16" t="n">
         <v>1</v>
       </c>
       <c r="G16" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" t="n">
+        <v>33</v>
+      </c>
+      <c r="I16" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" t="s">
         <v>141</v>
       </c>
-      <c r="H16" t="n">
-        <v>224</v>
-      </c>
-      <c r="I16" t="n">
-        <v>652</v>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="n">
+        <v>746877</v>
+      </c>
+      <c r="E17" t="n">
+        <v>894910</v>
+      </c>
+      <c r="F17" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="I17" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" t="n">
+        <v>751370</v>
+      </c>
+      <c r="E18" t="n">
+        <v>894910</v>
+      </c>
+      <c r="F18" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="I18" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" t="n">
+        <v>9683149</v>
+      </c>
+      <c r="E19" t="n">
+        <v>907020</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" t="n">
+        <v>558.45</v>
+      </c>
+      <c r="I19" t="n">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" t="n">
+        <v>69741</v>
+      </c>
+      <c r="E20" t="n">
+        <v>901236</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" t="n">
+        <v>207</v>
+      </c>
+      <c r="I20" t="n">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" t="s">
+        <v>141</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" t="n">
+        <v>69759</v>
+      </c>
+      <c r="E21" t="n">
+        <v>904280</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>116</v>
+      </c>
+      <c r="H21" t="n">
+        <v>138</v>
+      </c>
+      <c r="I21" t="n">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" t="n">
+        <v>69759</v>
+      </c>
+      <c r="E22" t="n">
+        <v>904280</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>119</v>
+      </c>
+      <c r="H22" t="n">
+        <v>138</v>
+      </c>
+      <c r="I22" t="n">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" t="s">
+        <v>141</v>
+      </c>
+      <c r="C23" t="s">
+        <v>128</v>
+      </c>
+      <c r="D23" t="n">
+        <v>360387</v>
+      </c>
+      <c r="E23" t="n">
+        <v>903682</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>133</v>
+      </c>
+      <c r="H23" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="I23" t="n">
+        <v>59.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>